<commit_message>
Start tsunami temperature rise calculation, correct nuclear concentrations in main report
</commit_message>
<xml_diff>
--- a/biological defence/данные для расчеты дозы до защиты.xlsx
+++ b/biological defence/данные для расчеты дозы до защиты.xlsx
@@ -138,15 +138,15 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -444,7 +444,7 @@
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -457,13 +457,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -493,25 +493,25 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>2.7943E-3</v>
+        <v>2.1052000000000002E-3</v>
       </c>
       <c r="D5">
-        <v>236.37</v>
+        <v>265.76</v>
       </c>
       <c r="E5">
-        <v>2.89</v>
+        <v>2.86</v>
       </c>
       <c r="F5">
         <f>C5*D5</f>
-        <v>0.66048869099999996</v>
+        <v>0.55947795200000006</v>
       </c>
       <c r="G5">
         <f>F5*E5</f>
-        <v>1.90881231699</v>
-      </c>
-      <c r="H5" s="3">
+        <v>1.6001069427200001</v>
+      </c>
+      <c r="H5" s="2">
         <f>(G5+G6)/(F5+F6)</f>
-        <v>2.9220405883685618</v>
+        <v>2.8892218551065882</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -519,28 +519,28 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>1.4698999999999999E-3</v>
+        <v>6.8223000000000003E-4</v>
       </c>
       <c r="D6">
-        <v>211.85</v>
+        <v>237.79</v>
       </c>
       <c r="E6">
         <v>2.99</v>
       </c>
       <c r="F6">
         <f>C6*D6</f>
-        <v>0.31139831499999998</v>
+        <v>0.16222747170000001</v>
       </c>
       <c r="G6">
         <f>E6*F6</f>
-        <v>0.93108096185</v>
+        <v>0.4850601403830001</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
@@ -562,16 +562,16 @@
         <f>566*0.001</f>
         <v>0.56600000000000006</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f>(B10*2*C10*PI() + 2 * PI() *C10^2)</f>
         <v>6.6360238612895639</v>
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
@@ -592,50 +592,50 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14">
-        <v>0.38512930000000001</v>
+        <v>0.4</v>
       </c>
       <c r="C14" s="1">
-        <v>1.459797E-2</v>
+        <v>2.2662359999999999E-2</v>
       </c>
       <c r="D14">
         <f>B14/C14</f>
-        <v>26.38238741414046</v>
-      </c>
-      <c r="E14">
+        <v>17.65041240188577</v>
+      </c>
+      <c r="E14" s="1">
         <f>(2.405/(C10*100))^2+(PI()/(B10*100))^2</f>
         <v>2.3894994550654443E-3</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f>1+E14*D14</f>
-        <v>1.063040700349414</v>
+        <v>1.0421756508159865</v>
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18">
-        <v>0.37260199999999999</v>
+        <v>0.3792084</v>
       </c>
       <c r="C18" s="1">
-        <v>9.8850370000000007E-2</v>
-      </c>
-      <c r="D18" s="6">
+        <v>0.112136</v>
+      </c>
+      <c r="D18" s="5">
         <f>B18/(C18+B18)</f>
-        <v>0.79032798159440787</v>
+        <v>0.77177718927904737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>